<commit_message>
Minor changes to 3DA forms
</commit_message>
<xml_diff>
--- a/forms/Form-3DA-multiple.xlsx
+++ b/forms/Form-3DA-multiple.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA3697E-FA8D-41AC-B84E-742E125B277D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF491C9-C93C-4DDE-A884-BF299B8A71A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="iDUEB36Tg6Fq49GBSSjSX4WaeYZypxEO4ytihSLd0MzE563An8wKW/Vc15EJLa1ODp4aG1zBQhFXgrBIWgpe9w==" workbookSaltValue="icTV95uKRvveyy8jCyTdwA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -673,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -936,6 +936,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1275,7 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2D41B5-AC8B-4133-9C08-EAF515BF72F5}">
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1635,7 +1638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C098252-FABC-4161-882E-794F98E79BC6}">
   <dimension ref="B1:Z55"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -1764,11 +1767,11 @@
       </c>
       <c r="H4" s="88"/>
       <c r="I4" s="89"/>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="88"/>
-      <c r="L4" s="89"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="90"/>
       <c r="M4" s="87" t="s">
         <v>38</v>
       </c>
@@ -3216,7 +3219,7 @@
       <c r="Z55" s="60"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="67IzirLU+Q+VZjPWCD1CSZku+Bs7km6f5yDyreJ7xf8wE1L8PP5hGsnHHXL7ffhnBTFaTMXTec5+k2oCVOeS1w==" saltValue="qgUKxSk7XyRG1OsmmNe4BQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="IeRD1x/JbnIwb/x3FjkSmnH0zRpVjkHoUKbeIXGFZABJvX/EKyhsXGe5u5VMA9WpXSQyh2bti3a5hM5TONlAOA==" saltValue="B7i6gBijKx8jAggo851Zbg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="B2:Z3"/>
     <mergeCell ref="B4:F4"/>

</xml_diff>